<commit_message>
updates to STG Card BOM
</commit_message>
<xml_diff>
--- a/notes/AVIELFSTGDISK0/AVIELFSTGDISK0-BOM.xlsx
+++ b/notes/AVIELFSTGDISK0/AVIELFSTGDISK0-BOM.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewwasson/Development/avi-elf-ii/notes/AVIELFSTGDISK0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{59722008-5FF5-7041-B4D2-A18EE3D479E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE7A305-0D49-A34A-B003-353BF009A624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30120" yWindow="3380" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="30120" yWindow="3380" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AVIELFSTGDISK0" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="174">
   <si>
     <t>C1, C2</t>
   </si>
@@ -130,9 +130,6 @@
     <t>Connector_Dsub:DSUB-9_Female_Horizontal_P2.77x2.84mm_EdgePinOffset9.90mm_Housed_MountingHolesOffset11.32mm</t>
   </si>
   <si>
-    <t xml:space="preserve"> ~</t>
-  </si>
-  <si>
     <t>J7, J8</t>
   </si>
   <si>
@@ -530,12 +527,27 @@
   </si>
   <si>
     <t>3M N7E50-M516RB-40 50 Position Card Connector CompactFlash® - Type I, II Surface Mount, Right Angle Gold</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/ftdi-future-technology-devices-international-ltd/FT232RL-TUBE/4006920</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/edac-inc/690-005-299-043/4312191</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/assmann-wsw-components/A-DF-09-A-KG-T2S/1241800</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/texas-instruments/MAX232N/277048</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/texas-instruments/SN74HC11N/376871</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1022,17 +1034,13 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
@@ -1391,11 +1399,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1409,114 +1417,114 @@
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B2" s="4"/>
+        <v>150</v>
+      </c>
+      <c r="B2"/>
       <c r="C2" s="1"/>
       <c r="D2"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>157</v>
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>156</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>160</v>
+      <c r="B4" t="s">
+        <v>159</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
-        <v>1</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>162</v>
+      <c r="A5" s="3">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>161</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
+      <c r="A6" s="3">
         <v>2</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>164</v>
+      <c r="B6" t="s">
+        <v>163</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
+      <c r="A7" s="3">
         <v>3</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>156</v>
+      <c r="B7" t="s">
+        <v>155</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>166</v>
+      <c r="B8" t="s">
+        <v>165</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1530,7 +1538,7 @@
     </row>
     <row r="10" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1542,16 +1550,16 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" t="s">
         <v>83</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>84</v>
-      </c>
-      <c r="E11" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1559,16 +1567,16 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" t="s">
         <v>87</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>88</v>
-      </c>
-      <c r="E12" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1576,16 +1584,16 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" t="s">
         <v>91</v>
       </c>
-      <c r="D13" t="s">
-        <v>92</v>
-      </c>
       <c r="E13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1593,16 +1601,16 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" t="s">
         <v>94</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>95</v>
-      </c>
-      <c r="E14" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1610,16 +1618,19 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" t="s">
         <v>98</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>99</v>
       </c>
-      <c r="E15" t="s">
-        <v>100</v>
+      <c r="F15" s="4" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1627,16 +1638,19 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" t="s">
         <v>102</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>103</v>
       </c>
-      <c r="E16" t="s">
-        <v>104</v>
+      <c r="F16" s="4" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1644,16 +1658,16 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C17" s="3">
         <v>16450</v>
       </c>
       <c r="D17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E17" t="s">
         <v>106</v>
-      </c>
-      <c r="E17" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1661,16 +1675,16 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
+        <v>107</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="D18" t="s">
         <v>109</v>
       </c>
-      <c r="D18" t="s">
-        <v>110</v>
-      </c>
       <c r="E18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1678,16 +1692,16 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="D19" t="s">
         <v>112</v>
       </c>
-      <c r="D19" t="s">
-        <v>113</v>
-      </c>
       <c r="E19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1695,16 +1709,16 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="D20" t="s">
         <v>115</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>116</v>
-      </c>
-      <c r="E20" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1712,16 +1726,16 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
+        <v>117</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="D21" t="s">
         <v>119</v>
       </c>
-      <c r="D21" t="s">
-        <v>120</v>
-      </c>
       <c r="E21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1729,16 +1743,16 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="D22" t="s">
         <v>122</v>
       </c>
-      <c r="D22" t="s">
-        <v>123</v>
-      </c>
       <c r="E22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1746,16 +1760,16 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
+        <v>123</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="D23" t="s">
         <v>125</v>
       </c>
-      <c r="D23" t="s">
-        <v>126</v>
-      </c>
       <c r="E23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1763,16 +1777,16 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
+        <v>126</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="D24" t="s">
         <v>128</v>
       </c>
-      <c r="D24" t="s">
-        <v>129</v>
-      </c>
       <c r="E24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1780,16 +1794,16 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
+        <v>129</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D25" t="s">
         <v>130</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D25" t="s">
-        <v>131</v>
-      </c>
       <c r="E25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1797,21 +1811,24 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
+        <v>131</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="D26" t="s">
         <v>133</v>
       </c>
-      <c r="D26" t="s">
-        <v>134</v>
-      </c>
       <c r="E26" t="s">
-        <v>85</v>
+        <v>84</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1823,7 +1840,7 @@
         <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>13</v>
@@ -1840,16 +1857,16 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="D30" t="s">
         <v>70</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>71</v>
-      </c>
-      <c r="E30" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1857,16 +1874,16 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
+        <v>134</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="D31" t="s">
         <v>136</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>137</v>
-      </c>
-      <c r="E31" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1878,7 +1895,7 @@
     </row>
     <row r="33" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -1886,11 +1903,11 @@
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="5">
+      <c r="A34" s="3">
         <v>8</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>149</v>
+      <c r="B34" t="s">
+        <v>148</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" t="s">
@@ -1900,8 +1917,8 @@
       <c r="F34" s="1"/>
     </row>
     <row r="35" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="5"/>
-      <c r="B35" s="4"/>
+      <c r="A35" s="3"/>
+      <c r="B35"/>
       <c r="C35" s="1"/>
       <c r="D35"/>
       <c r="E35" s="1"/>
@@ -1909,9 +1926,9 @@
     </row>
     <row r="36" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B36" s="4"/>
+        <v>151</v>
+      </c>
+      <c r="B36"/>
       <c r="C36" s="1"/>
       <c r="D36"/>
       <c r="E36" s="1"/>
@@ -1956,7 +1973,7 @@
         <v>13</v>
       </c>
       <c r="B39" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C39" s="3">
         <v>0.1</v>
@@ -1986,8 +2003,8 @@
       </c>
     </row>
     <row r="41" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="5"/>
-      <c r="B41" s="4"/>
+      <c r="A41" s="3"/>
+      <c r="B41"/>
       <c r="C41" s="1"/>
       <c r="D41"/>
       <c r="E41" s="1"/>
@@ -1995,9 +2012,9 @@
     </row>
     <row r="42" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B42" s="4"/>
+        <v>152</v>
+      </c>
+      <c r="B42"/>
       <c r="C42" s="1"/>
       <c r="D42"/>
       <c r="E42" s="1"/>
@@ -2008,16 +2025,16 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
+        <v>72</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="D43" t="s">
         <v>74</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>75</v>
-      </c>
-      <c r="E43" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -2025,16 +2042,16 @@
         <v>6</v>
       </c>
       <c r="B44" t="s">
+        <v>76</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>78</v>
-      </c>
       <c r="D44" t="s">
+        <v>74</v>
+      </c>
+      <c r="E44" t="s">
         <v>75</v>
-      </c>
-      <c r="E44" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -2042,21 +2059,21 @@
         <v>1</v>
       </c>
       <c r="B45" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C45" s="3">
         <v>470</v>
       </c>
       <c r="D45" t="s">
+        <v>79</v>
+      </c>
+      <c r="E45" t="s">
         <v>80</v>
       </c>
-      <c r="E45" t="s">
-        <v>81</v>
-      </c>
     </row>
     <row r="46" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="5"/>
-      <c r="B46" s="4"/>
+      <c r="A46" s="3"/>
+      <c r="B46"/>
       <c r="C46" s="1"/>
       <c r="D46"/>
       <c r="E46" s="1"/>
@@ -2064,9 +2081,9 @@
     </row>
     <row r="47" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B47" s="4"/>
+        <v>153</v>
+      </c>
+      <c r="B47"/>
       <c r="C47" s="1"/>
       <c r="D47"/>
       <c r="E47" s="1"/>
@@ -2097,16 +2114,16 @@
         <v>2</v>
       </c>
       <c r="B49" t="s">
+        <v>36</v>
+      </c>
+      <c r="C49" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="D49" t="s">
         <v>38</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>39</v>
-      </c>
-      <c r="E49" t="s">
-        <v>40</v>
       </c>
       <c r="F49" t="s">
         <v>4</v>
@@ -2117,16 +2134,16 @@
         <v>1</v>
       </c>
       <c r="B50" t="s">
+        <v>40</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="D50" t="s">
         <v>42</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>43</v>
-      </c>
-      <c r="E50" t="s">
-        <v>44</v>
       </c>
       <c r="F50" t="s">
         <v>4</v>
@@ -2137,16 +2154,16 @@
         <v>1</v>
       </c>
       <c r="B51" t="s">
+        <v>44</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C51" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="D51" t="s">
+        <v>42</v>
+      </c>
+      <c r="E51" t="s">
         <v>43</v>
-      </c>
-      <c r="E51" t="s">
-        <v>44</v>
       </c>
       <c r="F51" t="s">
         <v>4</v>
@@ -2157,16 +2174,16 @@
         <v>1</v>
       </c>
       <c r="B52" t="s">
+        <v>46</v>
+      </c>
+      <c r="C52" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C52" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="D52" t="s">
+        <v>42</v>
+      </c>
+      <c r="E52" t="s">
         <v>43</v>
-      </c>
-      <c r="E52" t="s">
-        <v>44</v>
       </c>
       <c r="F52" t="s">
         <v>4</v>
@@ -2177,16 +2194,16 @@
         <v>1</v>
       </c>
       <c r="B53" t="s">
+        <v>48</v>
+      </c>
+      <c r="C53" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C53" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="D53" t="s">
+        <v>42</v>
+      </c>
+      <c r="E53" t="s">
         <v>43</v>
-      </c>
-      <c r="E53" t="s">
-        <v>44</v>
       </c>
       <c r="F53" t="s">
         <v>4</v>
@@ -2197,16 +2214,16 @@
         <v>1</v>
       </c>
       <c r="B54" t="s">
+        <v>50</v>
+      </c>
+      <c r="C54" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C54" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="D54" t="s">
+        <v>42</v>
+      </c>
+      <c r="E54" t="s">
         <v>43</v>
-      </c>
-      <c r="E54" t="s">
-        <v>44</v>
       </c>
       <c r="F54" t="s">
         <v>4</v>
@@ -2217,16 +2234,16 @@
         <v>1</v>
       </c>
       <c r="B55" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D55" t="s">
+        <v>53</v>
+      </c>
+      <c r="E55" t="s">
         <v>54</v>
-      </c>
-      <c r="E55" t="s">
-        <v>55</v>
       </c>
       <c r="F55" t="s">
         <v>4</v>
@@ -2237,16 +2254,16 @@
         <v>1</v>
       </c>
       <c r="B56" t="s">
+        <v>55</v>
+      </c>
+      <c r="C56" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="D56" t="s">
         <v>57</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>58</v>
-      </c>
-      <c r="E56" t="s">
-        <v>59</v>
       </c>
       <c r="F56" t="s">
         <v>4</v>
@@ -2257,16 +2274,16 @@
         <v>1</v>
       </c>
       <c r="B57" t="s">
+        <v>59</v>
+      </c>
+      <c r="C57" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C57" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="D57" t="s">
+        <v>42</v>
+      </c>
+      <c r="E57" t="s">
         <v>43</v>
-      </c>
-      <c r="E57" t="s">
-        <v>44</v>
       </c>
       <c r="F57" t="s">
         <v>4</v>
@@ -2277,16 +2294,16 @@
         <v>1</v>
       </c>
       <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C58" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="D58" t="s">
+        <v>42</v>
+      </c>
+      <c r="E58" t="s">
         <v>43</v>
-      </c>
-      <c r="E58" t="s">
-        <v>44</v>
       </c>
       <c r="F58" t="s">
         <v>4</v>
@@ -2297,16 +2314,16 @@
         <v>2</v>
       </c>
       <c r="B59" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C59" s="3">
         <v>5</v>
       </c>
       <c r="D59" t="s">
+        <v>42</v>
+      </c>
+      <c r="E59" t="s">
         <v>43</v>
-      </c>
-      <c r="E59" t="s">
-        <v>44</v>
       </c>
       <c r="F59" t="s">
         <v>4</v>
@@ -2317,16 +2334,16 @@
         <v>1</v>
       </c>
       <c r="B60" t="s">
+        <v>64</v>
+      </c>
+      <c r="C60" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C60" s="3" t="s">
-        <v>66</v>
-      </c>
       <c r="D60" t="s">
+        <v>42</v>
+      </c>
+      <c r="E60" t="s">
         <v>43</v>
-      </c>
-      <c r="E60" t="s">
-        <v>44</v>
       </c>
       <c r="F60" t="s">
         <v>4</v>
@@ -2337,16 +2354,16 @@
         <v>1</v>
       </c>
       <c r="B61" t="s">
+        <v>66</v>
+      </c>
+      <c r="C61" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C61" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="D61" t="s">
+        <v>42</v>
+      </c>
+      <c r="E61" t="s">
         <v>43</v>
-      </c>
-      <c r="E61" t="s">
-        <v>44</v>
       </c>
       <c r="F61" t="s">
         <v>4</v>
@@ -2354,7 +2371,7 @@
     </row>
     <row r="62" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1"/>
-      <c r="B62" s="4"/>
+      <c r="B62"/>
       <c r="C62" s="1"/>
       <c r="D62"/>
       <c r="E62" s="1"/>
@@ -2362,9 +2379,9 @@
     </row>
     <row r="63" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B63" s="4"/>
+        <v>154</v>
+      </c>
+      <c r="B63"/>
       <c r="C63" s="1"/>
       <c r="D63"/>
       <c r="E63" s="1"/>
@@ -2381,10 +2398,10 @@
         <v>19</v>
       </c>
       <c r="D64" t="s">
-        <v>169</v>
-      </c>
-      <c r="F64" s="6" t="s">
         <v>168</v>
+      </c>
+      <c r="F64" s="4" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -2423,8 +2440,8 @@
       <c r="E66" t="s">
         <v>31</v>
       </c>
-      <c r="F66" t="s">
-        <v>4</v>
+      <c r="F66" s="4" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -2443,8 +2460,8 @@
       <c r="E67" t="s">
         <v>35</v>
       </c>
-      <c r="F67" t="s">
-        <v>36</v>
+      <c r="F67" s="4" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="68" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2456,7 +2473,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F64" r:id="rId1"/>
+    <hyperlink ref="F64" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F15" r:id="rId2" xr:uid="{0268D065-B238-3D40-9FFC-5AE357048F7D}"/>
+    <hyperlink ref="F66" r:id="rId3" xr:uid="{27FE616B-5BBF-E04E-A94A-C1238F364E08}"/>
+    <hyperlink ref="F67" r:id="rId4" xr:uid="{D79C575D-33F7-BF46-A694-55706719F3C5}"/>
+    <hyperlink ref="F26" r:id="rId5" xr:uid="{446FE69F-DCD6-E049-823C-EB26F11E52A6}"/>
+    <hyperlink ref="F16" r:id="rId6" xr:uid="{191D6095-32E5-D146-BA73-6527D66D4915}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>